<commit_message>
Coping methods for new files type were implemented. Card building method for attachments feature was done. Few bugs were fixed.
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3233D22F-FE5E-460F-83B4-2F81F67A6F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFF780-0114-4762-B25C-916BEAF94559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
+    <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,26 +287,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -632,8 +632,8 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,7 +641,7 @@
     <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="11"/>
+    <col min="4" max="4" width="9.140625" style="10"/>
     <col min="5" max="5" width="47.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
   </cols>
@@ -664,12 +664,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -679,7 +679,7 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
     </row>
@@ -689,7 +689,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>1</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -711,7 +711,7 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>1</v>
       </c>
     </row>
@@ -721,7 +721,7 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>1</v>
       </c>
     </row>
@@ -735,13 +735,13 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="9">
-        <v>0.6</v>
-      </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -755,7 +755,7 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -767,8 +767,8 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="10">
-        <v>0</v>
+      <c r="D10" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
       <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -791,10 +791,10 @@
       <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="10">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -808,7 +808,7 @@
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -830,7 +830,7 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>1</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>0</v>
       </c>
     </row>
@@ -852,8 +852,8 @@
       <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="10">
-        <v>0</v>
+      <c r="D17" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -863,10 +863,10 @@
       <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="10">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -883,7 +883,7 @@
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -891,7 +891,7 @@
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>0.5</v>
       </c>
     </row>
@@ -899,17 +899,17 @@
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Implementation of UI was started. DataGrid was added, loading main information inside dataGrid was done.
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFFF780-0114-4762-B25C-916BEAF94559}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93428A7-42CD-46C0-B129-68D04F9D28FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>UI</t>
   </si>
@@ -117,35 +117,89 @@
     <t>Коментарий</t>
   </si>
   <si>
-    <t>Необходимо добавить в шаблон 2 поля соответствующие дополнительным файлам связанным с документом. Полный список прикрепленных документов: 1)doc/docx/rtf 2)tif 3)pdf 4)вложения (файлы через ;)</t>
-  </si>
-  <si>
     <t>Копирование файлов вложений</t>
   </si>
   <si>
-    <t>Куда копировать файлы вложений? Видимо в N_attach</t>
-  </si>
-  <si>
     <t>Копирование pdf текстовых файлов связанных с документом в N_text директорию</t>
   </si>
   <si>
-    <t>Необходима реализация указания множественных файлов в одной ячейке, см. Файлы вложения</t>
-  </si>
-  <si>
     <t>Формирование дополнительной карточки для вложенных файлов в директории N_attach</t>
   </si>
   <si>
-    <t>При нескольких файлов вложения каким должно быть наполнение файла карточки? Или отдельно одна карточка для каждого файла?</t>
-  </si>
-  <si>
     <t>Формирование дополнительной карточки в папке N_attach с атрибутами 1: имя вложенного файла (из атрибута 7860:) 13: имя реального файла</t>
+  </si>
+  <si>
+    <t>Загрузка файла шаблона</t>
+  </si>
+  <si>
+    <t>Выбор файла шаблона и его загрузка в память.</t>
+  </si>
+  <si>
+    <t>Отображение загруженных данных шаблона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Загруженные данные </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Должен отображаться список документов со всеми загруженными атрибутами. </t>
+  </si>
+  <si>
+    <t>Отображать файлы связанные с документом</t>
+  </si>
+  <si>
+    <t>Запуск процесса обработки документов</t>
+  </si>
+  <si>
+    <t>По кнопке запуска должен начинаться процесс обработки документов и перенос файлов в нужные директории, процесс создания карточек и т.д.</t>
+  </si>
+  <si>
+    <t>Подкрашивать строки документов крассным цветом если в процессе обработки для данного файла произошла какая либо ошибка</t>
+  </si>
+  <si>
+    <t>Окно состояния документа</t>
+  </si>
+  <si>
+    <t>При выборе документа из списка должно открываться окно состояния документа</t>
+  </si>
+  <si>
+    <t>В окне состояния документа отображается текстовая информация по процессу обработки данного документа (логи), так же должно быть описание ошибок с данным документом если они были в процессе обработки</t>
+  </si>
+  <si>
+    <t>Окно настроек</t>
+  </si>
+  <si>
+    <t>Окно настроек должно открываться из меню приложения и содержать все настройки их AppConfig.xml с возможностью изменения и сохранения изменений</t>
+  </si>
+  <si>
+    <t>Указание номерации документов</t>
+  </si>
+  <si>
+    <t>В главном окне приложения, при загруженном шаблоне, необходи иметь возможность указать значения для номеров документов</t>
+  </si>
+  <si>
+    <t>Процесс обработки документов</t>
+  </si>
+  <si>
+    <t>Отображение процесса обработки</t>
+  </si>
+  <si>
+    <t>Необходимо отображать обрабатываемый документ и progress bar для суммарного процесса</t>
+  </si>
+  <si>
+    <t>Main Window</t>
+  </si>
+  <si>
+    <t>Doc State</t>
+  </si>
+  <si>
+    <t>Process Window</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +246,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,7 +335,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -287,12 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,7 +361,16 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -629,19 +694,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6578E407-3A24-41E4-8A8C-B6D277083C6D}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="10"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
     <col min="5" max="5" width="47.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
   </cols>
@@ -679,7 +744,7 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>1</v>
       </c>
     </row>
@@ -689,7 +754,7 @@
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>1</v>
       </c>
     </row>
@@ -699,7 +764,7 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
     </row>
@@ -711,7 +776,7 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
     </row>
@@ -721,11 +786,11 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -735,15 +800,11 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -755,7 +816,7 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>1</v>
       </c>
     </row>
@@ -767,7 +828,7 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>1</v>
       </c>
     </row>
@@ -777,26 +838,24 @@
         <v>3.3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3">
         <v>3.6</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="7">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -808,7 +867,7 @@
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>1</v>
       </c>
     </row>
@@ -819,7 +878,7 @@
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>1</v>
       </c>
     </row>
@@ -830,7 +889,7 @@
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="5">
         <v>1</v>
       </c>
     </row>
@@ -841,7 +900,7 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="7">
         <v>0</v>
       </c>
     </row>
@@ -850,25 +909,23 @@
         <v>3.5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4">
         <v>3.6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1</v>
+      </c>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
@@ -883,7 +940,7 @@
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -891,7 +948,7 @@
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="6">
         <v>0.5</v>
       </c>
     </row>
@@ -899,7 +956,7 @@
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>0</v>
       </c>
     </row>
@@ -911,11 +968,162 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
New functionality were implemented: - AppSettings window - Document Identity could be set inside excel template - Checking of overwriting document files.
Bugs fixed:
- Wrong parsing document number column when it contain double values
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93428A7-42CD-46C0-B129-68D04F9D28FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB926F41-EF64-453F-9B8E-07BC7E291A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>UI</t>
   </si>
@@ -193,6 +193,42 @@
   </si>
   <si>
     <t>Process Window</t>
+  </si>
+  <si>
+    <t>Баги</t>
+  </si>
+  <si>
+    <t>Номер документа</t>
+  </si>
+  <si>
+    <t>Если в колонке номер документа, только цифры, то они не попадают в карточку *.a2</t>
+  </si>
+  <si>
+    <t>Доп. Функционал</t>
+  </si>
+  <si>
+    <t>Редакции документов</t>
+  </si>
+  <si>
+    <t>Документ может ссылаться на уже существующий. В этом случае карточки для него должны создаваться в директории первоначального документа во сложенной папке.</t>
+  </si>
+  <si>
+    <t>Идентификаторы документов указываются в excel шаблоне</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Запрос на замену файла </t>
+  </si>
+  <si>
+    <t>Запрашивать у пользователя необходимость перезаписи файла при наличае такого же в output директории</t>
+  </si>
+  <si>
+    <t>Запрос на замену файла карточки</t>
+  </si>
+  <si>
+    <t>Запрашивать у пользователя необходимость перезаписи сформированной карточки, при наличае такой же</t>
+  </si>
+  <si>
+    <t>Не понятно, нужно ли это задавать через UI</t>
   </si>
 </sst>
 </file>
@@ -335,7 +371,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,11 +403,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -694,11 +733,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6578E407-3A24-41E4-8A8C-B6D277083C6D}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,12 +768,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -961,12 +1000,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -986,8 +1025,8 @@
       <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="7">
-        <v>0</v>
+      <c r="D27" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1003,127 +1042,200 @@
       <c r="D28" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="E28" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D33" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+    <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D41" s="7">
         <v>0</v>
       </c>
     </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="7">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A48:D48"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
- DocumentWindow implementation started. (Status document visualization) - DataGrid was changed to ListView/GridView - ListViewItems colarization functionallity started.
New functionality were implemented:
- AppSettings validation method.
- Core logger functionality.
- Checking of overwriting cards files.

Bugs fixed:
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB926F41-EF64-453F-9B8E-07BC7E291A5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11FAA5A-6D5B-4F0B-B68F-5FADE42B638E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>UI</t>
   </si>
@@ -153,9 +153,6 @@
     <t>По кнопке запуска должен начинаться процесс обработки документов и перенос файлов в нужные директории, процесс создания карточек и т.д.</t>
   </si>
   <si>
-    <t>Подкрашивать строки документов крассным цветом если в процессе обработки для данного файла произошла какая либо ошибка</t>
-  </si>
-  <si>
     <t>Окно состояния документа</t>
   </si>
   <si>
@@ -229,6 +226,21 @@
   </si>
   <si>
     <t>Не понятно, нужно ли это задавать через UI</t>
+  </si>
+  <si>
+    <t>Падение при загрузке шаблона template_1_30_2020_bug.xlsx</t>
+  </si>
+  <si>
+    <t>null refference exception при загрузке шаблона</t>
+  </si>
+  <si>
+    <t>Подкрашивать строки документов крассным цветом если в процессе обработки для данного файла произошла какая либо ошибка, зеленым если обработаны успешно</t>
+  </si>
+  <si>
+    <t>Реализовать строку состояния приложения. Отображать текущий статус загрузчика. Например, что необходимо загрузить шаблон или шаблон загружен</t>
+  </si>
+  <si>
+    <t>Строка состояния приложения</t>
   </si>
 </sst>
 </file>
@@ -403,14 +415,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="5" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -733,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6578E407-3A24-41E4-8A8C-B6D277083C6D}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,12 +780,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -979,33 +991,33 @@
       <c r="C21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="6">
-        <v>0.5</v>
+      <c r="D21" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="6">
-        <v>0.5</v>
+      <c r="D22" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1020,10 +1032,10 @@
     </row>
     <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D27" s="5">
         <v>1</v>
@@ -1031,211 +1043,239 @@
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D28" s="7">
         <v>0</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>65</v>
+      <c r="E28" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="C37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="7">
+      <c r="C38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="4" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0</v>
+      <c r="D41" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" s="5">
+        <v>49</v>
+      </c>
+      <c r="D42" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="7">
+      <c r="D44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="1" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D49" s="7">
+      <c r="D51" s="7">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A50:D50"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A40:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
New functionality were implemented:
Bugs fixed:
- Bug with loading documents with empty attributes
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11FAA5A-6D5B-4F0B-B68F-5FADE42B638E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439178F6-BB4C-4590-BE39-40B908423C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
+    <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -748,8 +748,8 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,8 +1244,8 @@
       <c r="C48" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="7">
-        <v>0</v>
+      <c r="D48" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Overwriting files process was reworked - New log messages were added - Document windows list views highlighting process was reworked
New functionality were implemented:
- Converting doc to mht
- Document state indicator was added

Bugs fixed:
</commit_message>
<xml_diff>
--- a/Docs/Plan_v1.xlsx
+++ b/Docs/Plan_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DocumentsMover\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439178F6-BB4C-4590-BE39-40B908423C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C1FBE2-7D00-4F20-8165-F56DEDB56826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="-120" windowWidth="27990" windowHeight="16440" xr2:uid="{FB553385-0B2B-4B7D-B3F7-CB717EE49FB4}"/>
   </bookViews>
@@ -383,7 +383,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -398,9 +398,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
@@ -748,8 +745,8 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +754,7 @@
     <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="4" max="4" width="9.140625" style="7"/>
     <col min="5" max="5" width="47.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.42578125" customWidth="1"/>
   </cols>
@@ -780,12 +777,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -854,8 +851,8 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -906,7 +903,7 @@
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="10"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -951,8 +948,8 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="7">
-        <v>0</v>
+      <c r="D16" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -976,7 +973,7 @@
       <c r="D18" s="5">
         <v>1</v>
       </c>
-      <c r="E18" s="10"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
@@ -1012,12 +1009,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1051,10 +1048,10 @@
       <c r="C28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="6">
         <v>0</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1076,17 +1073,17 @@
       <c r="C30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -1120,17 +1117,17 @@
       <c r="C34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="6">
-        <v>0.5</v>
+      <c r="D34" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -1153,17 +1150,17 @@
       <c r="C38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="7">
-        <v>0</v>
+      <c r="D38" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
     </row>
     <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1189,7 +1186,7 @@
       <c r="C42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1219,12 +1216,12 @@
       <c r="D45"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1249,12 +1246,12 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
@@ -1263,7 +1260,7 @@
       <c r="C51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>